<commit_message>
Updaing mistake in template
</commit_message>
<xml_diff>
--- a/_raw/antigenic_map_template.xlsx
+++ b/_raw/antigenic_map_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oliv4107.NEXT\Documents\R\Bachelor\Antigenic-Mapping-of-NA\_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B460243-E4B6-418B-8946-8A6A9F4DAB45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAB9396-A942-40F3-AF29-2BCEF32212C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AntigenicMappingTemplate_ATM_" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="74">
   <si>
     <t>Made by;                                                                OLSE &amp; MAOJ, 2024</t>
   </si>
@@ -1143,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:JZ263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AI11" sqref="AI11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
@@ -2740,6 +2740,9 @@
         <v>17</v>
       </c>
       <c r="AE9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -63103,18 +63106,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63136,18 +63139,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B7222CD-4E52-4DCB-A6D9-A689C06F8147}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19DF177C-8C67-469D-A144-41DE0BEB0C8E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B7222CD-4E52-4DCB-A6D9-A689C06F8147}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>